<commit_message>
Addede banred, backsub and loads
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2025-a\Analisis Matricial Estructuras\Calculadora-Cerchas-Corregido\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688D1CE1-08F3-457F-A5AF-13F75DD412FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5521B8B-5908-4D49-BDF0-207029410693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="11010" windowHeight="12885" firstSheet="2" activeTab="3" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="11010" windowHeight="12885" firstSheet="2" activeTab="4" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,10 +959,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED023E19-6C40-4444-B782-2C29E3B94B11}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,6 +1034,20 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>-10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added rigid_jointed.py, needs fix on gamma
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2025-a\Analisis Matricial Estructuras\Calculadora-Cerchas-Corregido\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D5A6F1-4208-4928-AE4E-5256B17C7FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0FACBD-D424-4545-985D-293459857FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="5" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
@@ -41,14 +41,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>DIM</t>
   </si>
   <si>
-    <t>EA</t>
-  </si>
-  <si>
     <t>Conectiv_i</t>
   </si>
   <si>
@@ -83,14 +80,58 @@
   </si>
   <si>
     <t>PROPS</t>
+  </si>
+  <si>
+    <t>Iy (cm^4)</t>
+  </si>
+  <si>
+    <t>Iz (cm^4)</t>
+  </si>
+  <si>
+    <t>vx</t>
+  </si>
+  <si>
+    <t>vy</t>
+  </si>
+  <si>
+    <t>vz</t>
+  </si>
+  <si>
+    <t>ϑx</t>
+  </si>
+  <si>
+    <t>ϑy</t>
+  </si>
+  <si>
+    <t>ϑz</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>PROP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -106,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -142,14 +183,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,249 +553,285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>3</v>
+      <c r="C4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5">
         <v>3</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6">
         <v>4</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7">
         <v>5</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8">
         <v>6</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9">
         <v>7</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5</v>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="1">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="1">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
-        <v>7</v>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1">
-        <v>7</v>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14">
         <v>8</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>8</v>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
-      <c r="B16" s="1">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1">
-        <v>8</v>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1">
-        <v>8</v>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1">
-        <v>8</v>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
-      <c r="B19" s="1">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1">
-        <v>8</v>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1">
-        <v>8</v>
-      </c>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1">
-        <v>8</v>
-      </c>
+      <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -735,23 +840,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="A14" sqref="A14:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -770,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -778,10 +883,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -789,10 +894,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -800,73 +905,194 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -900,26 +1126,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -929,8 +1164,17 @@
       <c r="C2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.91</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -940,17 +1184,20 @@
       <c r="C3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10</v>
-      </c>
+      <c r="D3" s="1">
+        <v>1320</v>
+      </c>
+      <c r="E3" s="1">
+        <v>101</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -962,23 +1209,23 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,83 +1305,221 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88FFCBC-CADB-4BE8-A2F4-8F5C5886CB8B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arreglado ndim y rigid_jointed
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2025-a\Analisis Matricial Estructuras\Calculadora-Cerchas-Corregido\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\PycharmProjects\CalculadoraCerchasFinal\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0FACBD-D424-4545-985D-293459857FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABDC6BF-140A-4CDF-A5AB-0A6A1F24B0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="5" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>DIM</t>
   </si>
@@ -64,15 +64,6 @@
     <t>A (cm^2)</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>NODO</t>
   </si>
   <si>
@@ -109,14 +100,38 @@
     <t>v</t>
   </si>
   <si>
-    <t>PROP</t>
+    <t>etype</t>
+  </si>
+  <si>
+    <t>Fx</t>
+  </si>
+  <si>
+    <t>Fy</t>
+  </si>
+  <si>
+    <t>Fz</t>
+  </si>
+  <si>
+    <t>Mx</t>
+  </si>
+  <si>
+    <t>My</t>
+  </si>
+  <si>
+    <t>Mz</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,14 +145,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -194,31 +201,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,14 +549,14 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -577,10 +570,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,225 +581,105 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>14</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>15</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>13</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>15</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>9</v>
-      </c>
-      <c r="C15">
-        <v>11</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>13</v>
-      </c>
-      <c r="C19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -843,7 +716,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,29 +737,29 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -894,150 +767,78 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>4</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>4</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>7.5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1">
-        <v>4</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,35 +927,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1165,16 +972,23 @@
         <v>10</v>
       </c>
       <c r="D2" s="1">
-        <v>1.91</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>1.91</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1185,16 +999,23 @@
         <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>1320</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>101</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
@@ -1206,31 +1027,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED023E19-6C40-4444-B782-2C29E3B94B11}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -1239,63 +1069,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-10</v>
+        <v>-100</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1305,221 +1088,82 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88FFCBC-CADB-4BE8-A2F4-8F5C5886CB8B}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6"/>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>